<commit_message>
Save into .xls File
</commit_message>
<xml_diff>
--- a/laptop_data.xlsx
+++ b/laptop_data.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:Q19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,7 +424,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Product Name</t>
+          <t>Name</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -445,6 +445,1472 @@
       <c r="E1" t="inlineStr">
         <is>
           <t>Availability</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Graphics Coprocessor</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Ram Memory Installed Size</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Operating System</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>CPU Speed</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>Special Feature</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>Color</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>Model Name</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>Hard Disk Size</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>Graphics Card Description</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>Screen Size</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>Brand</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>CPU Model</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Apple 2020 MacBook Air Laptop M1 Chip, 13" Retina Display, 8GB RAM, 256GB SSD Storage, Backlit Keyboard, FaceTime HD Camera, Touch ID. Works with iPhone/iPad; Space Gray</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>$703.99</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>4.8 out of 5 stars</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>19,617 ratings</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>In Stock</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>8 GB</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Mac OS</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Backlit Keyboard</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Space Gray</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>MacBook Air</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>256 GB</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>Integrated</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>13.3 Inches</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>Apple</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Apple 2023 MacBook Air Laptop with M2 chip: 15.3-inch Liquid Retina Display, 8GB Unified Memory, 256GB SSD Storage, 1080p FaceTime HD Camera, Touch ID. Works with iPhone/iPad; Midnight</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Page 1 of 1</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>4.3 out of 5 stars</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>17 ratings</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Not available</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>8 GB</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Mac OS</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Apple M2 Chip, Liquid Retina display with True Tone, Solid-state drive storage, Backlit Magic Keyboard with Touch ID, Unified Memory</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Midnight</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>MacBook Air</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>256 GB</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>Integrated</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>15.3 Inches</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>Apple</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Samsung Chromebook 4 (2021 Model) 11.6" Intel UHD Graphics 600, Intel Celeron Processor N4020, 4GB, 16GB- Wi-Fi - Satin Gray- (XE310XBA-KB1US)</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Page 1 of 1</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>4.4 out of 5 stars</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>259 ratings</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Intel Celeron Processor N4000</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>4 GB</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Chrome OS</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Anti Glare Coating</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Satin Gray</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>Chromebook 4</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>Integrated</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>11.6 Inches</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>SAMSUNG</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>Celeron N3450</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>ASUS G614JV-AS73 ROG Strix G16 (2023) Gaming Laptop, 16â€ 16:10 FHD 165Hz, GeForce RTX 4060, Intel Core i7-13650HX, 16GB DDR5, 512GB PCIe SSD, Wi-Fi 6E, Windows 11, G614JV-AS73, Eclipse Gray</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>$1,229.99</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>4.4 out of 5 stars</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>242 ratings</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Not available</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>16 GB</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Windows 11 Home</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Anti Glare Coating</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Eclipse Gray</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>ROG Strix G16</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>512 GB</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>Dedicated</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>16 Inches</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>ASUS</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>Intel Core i7</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>ASUS FX506HF-ES51 TUF Gaming F15 Gaming Laptop, 15.6â€ 144Hz FHD Display, Intel Core i5-11400H Processor, GeForce RTX 2050, 8GB DDR4 RAM, 512GB PCIe SSD Gen 3, Wi-Fi 6, Windows 11, FX506HF-ES51</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>$699.99</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>4.6 out of 5 stars</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>1,651 ratings</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Not available</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>8 GB</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Windows 11 Home</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Anti Glare Coating</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Graphite Black</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>FX506HF-ES51</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>256 GB</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>Dedicated</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>15.6 Inches</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>ASUS</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>Core i5</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Lenovo - 2022 - IdeaPad Flex 5i - 2-in-1 Chromebook Laptop Computer - Intel Core i3-1115G4 - 13.3" FHD Touch Display - 8GB Memory - 128GB Storage - Chrome OS</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>$397.99</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>4.4 out of 5 stars</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>1,068 ratings</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>In Stock</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>8 GB</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Chrome OS</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Anti Glare Coating</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Abyss Blue</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>IdeaPad Flex 5i Chromebook</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>128 GB</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>Integrated</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>13.3</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>Lenovo</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>Core i3</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Acer 2023 15" HD Premium Chromebook, Intel Celeron N Processor 2.78GHz Turbo Speed, 4GB Ram, 64GB SSD, Ultra-Fast WiFi Up to 1700 Mbps, Full Size Keyboard, Chrome OS, Arctic Silver Color-(Renewed)</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>$178.99</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>5.0 out of 5 stars</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>6 ratings</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>In Stock.</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Intel</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>4 GB</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Chrome OS</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>2.6 GHz</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>Acer 15" Chromebook</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>64 GB</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>Integrated</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>15 Inches</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>Acer</t>
+        </is>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>Celeron N</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Lenovo 2022 Newest Ideapad 3 Laptop, 15.6" HD Touchscreen, 11th Gen Intel Core i3-1115G4 Processor, 8GB DDR4 RAM, 256GB PCIe NVMe SSD, HDMI, Webcam, Wi-Fi 5, Bluetooth, Windows 11 Home, Almond</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>$422.99</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>4.3 out of 5 stars</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>3,320 ratings</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>In Stock</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>20 GB</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Windows 11</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>Anti Glare Coating</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>Almond</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>IdeaPad 3 81X800ENUS</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>256 GB</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>Integrated</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>15.6 Inches</t>
+        </is>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>Lenovo</t>
+        </is>
+      </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>Core i3</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Acer Aspire 3 A315-24P-R7VH Slim Laptop | 15.6" Full HD IPS Display | AMD Ryzen 3 7320U Quad-Core Processor | AMD Radeon Graphics | 8GB LPDDR5 | 128GB NVMe SSD | Wi-Fi 6 | Windows 11 Home in S Mode</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>$329.99</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>4.5 out of 5 stars</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>35,974 ratings</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>In Stock</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>AMD Radeon Graphics</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>8 GB</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Windows 11 S</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>Silver</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>A315-24P-R7VH</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>128 GB</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>Integrated</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>15.6 Inches</t>
+        </is>
+      </c>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>acer</t>
+        </is>
+      </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>Ryzen 3</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Acer Aspire 5 A515-46-R3UB | 15.6" Full HD IPS Display | AMD Ryzen 3 3350U Quad-Core Mobile Processor | 4GB DDR4 | 128GB NVMe SSD | WiFi 6 | Backlit KB | FPR | Amazon Alexa | Windows 11 Home in S mode</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Page 1 of 1</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>4.5 out of 5 stars</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>2,724 ratings</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>4 GB</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Windows 11</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>Fingerprint Reader, Backlit Keyboard</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>Silver</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>Aspire 5</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>128 GB</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>Integrated</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>15.6 Inches</t>
+        </is>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>acer</t>
+        </is>
+      </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>Ryzen 3 3350U</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Lenovo IdeaPad Gaming 3 - (2022) - Essential Gaming Laptop Computer - 15.6" FHD - 120Hz - AMD Ryzen 5 6600H - NVIDIA GeForce RTX 3050 - 8GB DDR5 RAM - 256GB NVMe Storage - Windows 11 Home</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>$679.99</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>4.3 out of 5 stars</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>792 ratings</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>In Stock</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>8 GB</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Windows 11 Home</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>Anti Glare Coating</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>Onyx Grey</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>IdeaPad Gaming 3</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>256 GB</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>Dedicated</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>15.6</t>
+        </is>
+      </c>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>Lenovo</t>
+        </is>
+      </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>Ryzen 5</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Acer Aspire 5 A515-56-347N Slim Laptop - 15.6" Full HD IPS Display - 11th Gen Intel i3-1115G4 Dual Core Processor - 8GB DDR4 - 128GB NVMe SSD - WiFi 6 - Amazon Alexa - Windows 11 Home in S Mode</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>$364.46</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>4.3 out of 5 stars</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>2,417 ratings</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>In Stock</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>8 GB</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Windows 11 S</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>Amazon Alexa</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>Silver</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>A515-56-347N</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>128 GB</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>Integrated</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>15.6 Inches</t>
+        </is>
+      </c>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>acer</t>
+        </is>
+      </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>Core I3 1115G4</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Dell 2022 Newest Inspiron 15 Laptop, 15.6" HD Display, Intel Celeron N4020 Processor, 16GB DDR4 RAM, 1TB PCIe SSD, Webcam, HDMI, Wi-Fi, Bluetooth, Windows 11 Home, Black</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>$429.00</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>4.1 out of 5 stars</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>294 ratings</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Not available</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>16 GB</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Windows 11 Home</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr"/>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>Anti Glare Coating</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>Black</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>Inspiron</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>1 TB</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>Integrated</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>15.6 Inches</t>
+        </is>
+      </c>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>Dell</t>
+        </is>
+      </c>
+      <c r="Q14" t="inlineStr">
+        <is>
+          <t>Celeron N4020</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Apple 2022 MacBook Pro Laptop with M2 chip: 13-inch Retina Display, 8GB RAM, 256GB ​​​​​​​SSD ​​​​​​​Storage, Touch Bar, Backlit Keyboard, FaceTime HD Camera. Works with iPhone and iPad; Silver</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>$1,011.08</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>4.7 out of 5 stars</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>1,059 ratings</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Not available</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>8 GB</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>Mac OS</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr"/>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>Backlit Keyboard</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>Silver</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>MacBook Pro</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>256 GB</t>
+        </is>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>Integrated</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>13.3 Inches</t>
+        </is>
+      </c>
+      <c r="P15" t="inlineStr">
+        <is>
+          <t>Apple</t>
+        </is>
+      </c>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Samsung Chromebook 4 Chrome OS 11.6" HD Intel Celeron Processor N4000 4GB RAM 32GB eMMC Gigabit Wi-Fi - XE310XBA-K01US</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>$152.00</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>4.4 out of 5 stars</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>2,601 ratings</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>In Stock</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Intel Celeron Processor N4000</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>4 GB</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Chrome OS</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr"/>
+      <c r="J16" t="inlineStr"/>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>Platinum Titan</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>Chromebook 4</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>32 GB</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>Integrated</t>
+        </is>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>11.6 Inches</t>
+        </is>
+      </c>
+      <c r="P16" t="inlineStr">
+        <is>
+          <t>SAMSUNG</t>
+        </is>
+      </c>
+      <c r="Q16" t="inlineStr">
+        <is>
+          <t>Celeron N3450</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Acer Aspire 1 A115-32-C96U Slim Laptop | 15.6" Full HD Display | Intel Celeron N4500 Processor | 4GB DDR4 | 128GB eMMC | WiFi 5 | Microsoft 365 Personal 1-Year Subscription | Windows 11 Home in S mode</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>$229.99</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>3.6 out of 5 stars</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>64 ratings</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>In Stock</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Intel UHD Graphics</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>4 GB</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>Windows 11 S</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>2.8 GHz</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr"/>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>Silver</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>A115-32-C96U</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr"/>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>Integrated</t>
+        </is>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>15.6 Inches</t>
+        </is>
+      </c>
+      <c r="P17" t="inlineStr">
+        <is>
+          <t>Acer</t>
+        </is>
+      </c>
+      <c r="Q17" t="inlineStr">
+        <is>
+          <t>Celeron N</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>HP 2022 Newest Laptops for College Student &amp; Business, 15.6 inch HD Computer, Intel Pentium Silver N5000, 16GB RAM, 1TB SSD, Office 365 1-Year, Fast Charge, Light-Weight, Windows 11, ROKC HDMI Cable</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>$519.99</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>4.5 out of 5 stars</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>54 ratings</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Not available</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Intel UHD Graphics 605</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>16 GB</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>Windows 11</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr"/>
+      <c r="J18" t="inlineStr"/>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>Red</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>HP Laptops</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>1000 GB</t>
+        </is>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>Integrated</t>
+        </is>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>15.6 Inches</t>
+        </is>
+      </c>
+      <c r="P18" t="inlineStr">
+        <is>
+          <t>HP</t>
+        </is>
+      </c>
+      <c r="Q18" t="inlineStr">
+        <is>
+          <t>Pentium N5000</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Lenovo 3i Chromebook - 2023 - Everyday Notebook - Chrome OS - 15.6" Full HD - 8GB Memory - 64GB Storage - Intel Celeron N4500 - Abyss Blue</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>$299.99</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>4.4 out of 5 stars</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>1,068 ratings</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>In Stock</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr"/>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>8 GB</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>Chrome OS</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr"/>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>Narrow</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>Blue</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>IdeaPad 3</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>64 GB</t>
+        </is>
+      </c>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>Integrated</t>
+        </is>
+      </c>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>15.6 Inches</t>
+        </is>
+      </c>
+      <c r="P19" t="inlineStr">
+        <is>
+          <t>Lenovo</t>
+        </is>
+      </c>
+      <c r="Q19" t="inlineStr">
+        <is>
+          <t>Celeron P4500</t>
         </is>
       </c>
     </row>

</xml_diff>